<commit_message>
Neat 336 asset loader introduce asset rule analysis module (#517)
* added serializer for rules

* allow dumping AssetRules as info rules

* allow conversion of asset rules to info rules

* allow conversion of asset rules to info rules

* some methods defs

* enable conversion from assetrules to info and dms rules

* add converter from info to asset rules

* added test

* not implemented

* bump version

* bump version

* bump version

* base analyzer

* resolving rules

* added asset expert analysis

* update method

* fix small

* updated changelog

* updated changelog

* added test

* remove dead code
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/asset-architect-jimbo.xlsx
+++ b/docs/artifacts/rules/asset-architect-jimbo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5B91EE-D427-A847-973D-0DE44BBCB3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B382097-90C1-3A4E-B63B-910C1DE15BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -596,7 +596,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,6 +737,14 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -836,7 +844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -907,28 +915,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -949,15 +942,25 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1267,7 +1270,7 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1301,7 +1304,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="39" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1370,7 +1373,7 @@
       <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="20"/>
@@ -9164,13 +9167,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -9194,19 +9197,19 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="35" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10391,8 +10394,8 @@
   </sheetPr>
   <dimension ref="A1:W925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="H41" sqref="H40:H41"/>
+    <sheetView topLeftCell="D1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10403,25 +10406,26 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="8" customWidth="1"/>
-    <col min="7" max="8" width="62.1640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="80.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="62.1640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="23" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -10469,446 +10473,446 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="25">
         <v>1</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="25">
         <v>1</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="25">
         <v>1</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="25">
         <v>1</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="25">
         <v>1</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="25">
         <v>1</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="28"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="25">
         <v>1</v>
       </c>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="25">
         <v>1</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9" s="25">
         <v>1</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>1</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="25">
         <v>1</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="25">
         <v>1</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="25">
         <v>1</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="25">
         <v>1</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="25">
         <v>1</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="25">
         <v>1</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="25">
         <v>1</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>1</v>
       </c>
-      <c r="F14" s="29">
+      <c r="F14" s="25">
         <v>1</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="25">
         <v>1</v>
       </c>
-      <c r="F15" s="29">
+      <c r="F15" s="25">
         <v>1</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>1</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="25">
         <v>1</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="25">
         <v>1</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="25">
         <v>1</v>
       </c>
-      <c r="F18" s="29">
+      <c r="F18" s="25">
         <v>1</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="25">
         <v>1</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="25">
         <v>1</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
@@ -17264,7 +17268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEC69AD-6A47-8A49-AB04-004D0BC3921D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -17275,130 +17279,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="34" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="30" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="32" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="32" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="32" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="32" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="32" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="32" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="30" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wrapping up asset loader (#551)
* scoping of asset loader

* add write_to_file

* use cameCase for asset properties

* fix failing tests

* fix test

* making sure we do not create asset whose parent does not exist

* making sure we do not create asset whose parent does not exist

* orphage test

* bump version add changelog

* update change log [skip ci]

* Update cognite/neat/graph/loaders/_rdf2asset.py

Co-authored-by: Anders Albert <60234212+doctrino@users.noreply.github.com>

* fix error

* fix error

* use upserted instead of create

---------

Co-authored-by: Anders Albert <60234212+doctrino@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/asset-architect-jimbo.xlsx
+++ b/docs/artifacts/rules/asset-architect-jimbo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/docs/artifacts/rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B382097-90C1-3A4E-B63B-910C1DE15BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5DE7BF-E20E-8A42-92E6-3C4E87F9E920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="104">
   <si>
     <t>Data Model Properties</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Data model classes</t>
-  </si>
-  <si>
-    <t>Parent Class</t>
   </si>
   <si>
     <t>role</t>
@@ -586,10 +583,10 @@
     <t>Asset(property=name)</t>
   </si>
   <si>
-    <t>Asset(property=parent_external_id), Relationship(label=belongsTo)</t>
+    <t>Relationship(label=connectsTo)</t>
   </si>
   <si>
-    <t>Relationship(label=connectsTo)</t>
+    <t>Asset(property=parentExternalId), Relationship(label=belongsTo)</t>
   </si>
 </sst>
 </file>
@@ -951,6 +948,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -960,7 +958,6 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1289,34 +1286,34 @@
   <sheetData>
     <row r="1" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="16" t="s">
+    </row>
+    <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="B3" s="16" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="18"/>
@@ -1342,10 +1339,10 @@
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -1371,10 +1368,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -1400,10 +1397,10 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -1429,10 +1426,10 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
@@ -1458,7 +1455,7 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="16">
         <v>45331</v>
@@ -1487,7 +1484,7 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="16">
         <v>45331</v>
@@ -1516,10 +1513,10 @@
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>28</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -1545,10 +1542,10 @@
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -9150,30 +9147,29 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Y998"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="25" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:25" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -9194,9 +9190,8 @@
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
       <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-    </row>
-    <row r="2" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -9204,215 +9199,186 @@
         <v>3</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="35" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="12"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="14"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="14"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="14"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="29" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10381,7 +10347,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10394,8 +10360,8 @@
   </sheetPr>
   <dimension ref="A1:W925"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10414,18 +10380,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -10460,10 +10426,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -10474,10 +10440,10 @@
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
@@ -10490,20 +10456,20 @@
         <v>1</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
@@ -10516,20 +10482,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
@@ -10542,20 +10508,20 @@
         <v>1</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
@@ -10568,20 +10534,20 @@
         <v>1</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
@@ -10594,20 +10560,20 @@
         <v>1</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
@@ -10620,24 +10586,24 @@
         <v>1</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="25">
         <v>1</v>
@@ -10646,7 +10612,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>103</v>
@@ -10656,10 +10622,10 @@
     </row>
     <row r="10" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
@@ -10672,20 +10638,20 @@
         <v>1</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
@@ -10698,24 +10664,24 @@
         <v>1</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="25">
         <v>1</v>
@@ -10724,7 +10690,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="26" t="s">
         <v>103</v>
@@ -10737,7 +10703,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10" t="s">
@@ -10750,10 +10716,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
@@ -10763,7 +10729,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10" t="s">
@@ -10776,10 +10742,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
@@ -10789,11 +10755,11 @@
         <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" s="25">
         <v>1</v>
@@ -10802,7 +10768,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="26" t="s">
         <v>103</v>
@@ -10815,11 +10781,11 @@
         <v>11</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="25">
         <v>1</v>
@@ -10828,20 +10794,20 @@
         <v>10</v>
       </c>
       <c r="G16" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
@@ -10854,20 +10820,20 @@
         <v>1</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
@@ -10880,20 +10846,20 @@
         <v>1</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
@@ -10906,7 +10872,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>103</v>
@@ -17268,7 +17234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEC69AD-6A47-8A49-AB04-004D0BC3921D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -17280,123 +17246,123 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="C1" s="34" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>70</v>
-      </c>
       <c r="C2" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>72</v>
-      </c>
       <c r="C3" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>74</v>
-      </c>
       <c r="C4" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="C5" s="32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>78</v>
-      </c>
       <c r="C6" s="32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>80</v>
-      </c>
       <c r="C7" s="32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>82</v>
-      </c>
       <c r="C8" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="29" t="s">
-        <v>86</v>
-      </c>
       <c r="C10" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>88</v>
-      </c>
       <c r="C11" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>